<commit_message>
fixed sorting orders bug: added production time twice
</commit_message>
<xml_diff>
--- a/Prod_Plan_1.xlsx
+++ b/Prod_Plan_1.xlsx
@@ -19,37 +19,37 @@
     <t>Machines</t>
   </si>
   <si>
-    <t>Order 4 - 20</t>
-  </si>
-  <si>
-    <t>Order 3 - 52</t>
-  </si>
-  <si>
-    <t>Order 10 - 174</t>
-  </si>
-  <si>
-    <t>Order 2 - 39</t>
-  </si>
-  <si>
-    <t>Order 5 - 118</t>
-  </si>
-  <si>
-    <t>Order 6 - 26</t>
-  </si>
-  <si>
-    <t>Order 9 - 100</t>
-  </si>
-  <si>
-    <t>Order 1 - 261</t>
+    <t>Order 9 - 48</t>
+  </si>
+  <si>
+    <t>Order 3 - 74</t>
+  </si>
+  <si>
+    <t>Order 4 - 80</t>
+  </si>
+  <si>
+    <t>Order 10 - 150</t>
+  </si>
+  <si>
+    <t>Order 5 - 40</t>
+  </si>
+  <si>
+    <t>Order 2 - 79</t>
+  </si>
+  <si>
+    <t>Order 1 - 61</t>
+  </si>
+  <si>
+    <t>Order 6 - 87</t>
   </si>
   <si>
     <t>Order 8 - 34</t>
   </si>
   <si>
-    <t>Order 7 - 125</t>
-  </si>
-  <si>
-    <t>make span: 261</t>
+    <t>Order 7 - 91</t>
+  </si>
+  <si>
+    <t>make span: 150</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -407,16 +407,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>143</v>
+        <v>71</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="D4">
-        <v>136</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -438,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -452,10 +452,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -465,8 +465,10 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>